<commit_message>
Changes made for demo
These are test changes made for the github demo
</commit_message>
<xml_diff>
--- a/tracking_tables/excluded_structures_tracking_table_template.xlsx
+++ b/tracking_tables/excluded_structures_tracking_table_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cwffcf.sharepoint.com/sites/Conservation-General/Shared Documents/Freshwater/Fish Passage/General WCRP/Internal WCRP workshop (2023)/Table and list templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\wcrp-github-training\tracking_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{8E96DE89-45B0-430D-ACC1-92D82D1ACB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{390A770E-7BB7-40BB-B65F-24B759D0D157}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C90270-3FE6-4B5F-B32E-8DC128AD42F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
+    <workbookView xWindow="2020" yWindow="380" windowWidth="15980" windowHeight="8900" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Excluded structures" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Internal Name</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Informal assessment</t>
+  </si>
+  <si>
+    <t>for testing</t>
   </si>
 </sst>
 </file>
@@ -175,10 +178,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,9 +479,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B487CB3-A96E-4BA8-A6AF-7460CE78FFCD}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -666,14 +665,40 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -767,25 +792,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1067,22 +1079,31 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
-    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1108,9 +1129,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
+    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Changes made for demo"
This reverts commit f1196e9136378430f4e1b827a575983060b6f7c0.
</commit_message>
<xml_diff>
--- a/tracking_tables/excluded_structures_tracking_table_template.xlsx
+++ b/tracking_tables/excluded_structures_tracking_table_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\wcrp-github-training\tracking_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cwffcf.sharepoint.com/sites/Conservation-General/Shared Documents/Freshwater/Fish Passage/General WCRP/Internal WCRP workshop (2023)/Table and list templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C90270-3FE6-4B5F-B32E-8DC128AD42F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{8E96DE89-45B0-430D-ACC1-92D82D1ACB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{390A770E-7BB7-40BB-B65F-24B759D0D157}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="380" windowWidth="15980" windowHeight="8900" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Excluded structures" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Internal Name</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Informal assessment</t>
-  </si>
-  <si>
-    <t>for testing</t>
   </si>
 </sst>
 </file>
@@ -178,6 +175,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,9 +480,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B487CB3-A96E-4BA8-A6AF-7460CE78FFCD}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -665,40 +666,14 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -792,12 +767,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1079,31 +1067,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
+    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1129,13 +1108,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
-    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Removing demo entries to create blank slate
</commit_message>
<xml_diff>
--- a/tracking_tables/excluded_structures_tracking_table_template.xlsx
+++ b/tracking_tables/excluded_structures_tracking_table_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\wcrp-github-training\tracking_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nWright\Documents\GitHub\wcrp-github-training\tracking_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1529FB-9581-4A88-A15D-940AC4EED058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F207639A-A570-4A10-AACD-6D7B403B5DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="380" windowWidth="15980" windowHeight="8900" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Excluded structures" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Internal Name</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Informal assessment</t>
-  </si>
-  <si>
-    <t>for demo</t>
   </si>
 </sst>
 </file>
@@ -479,9 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B487CB3-A96E-4BA8-A6AF-7460CE78FFCD}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -531,39 +528,15 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
@@ -792,15 +765,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F2D6C6860AC114F8559403465E77CC4" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a456bade4bd732af03e24b44c1c2ca9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="411171ba-2276-4762-a69b-ae0a1d76a912" xmlns:ns3="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="630d1ab75a49860de5f9d74b152c7650" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1078,6 +1042,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1101,14 +1074,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B063947-0EE7-419B-A8E4-FA2F4F0C123E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1128,6 +1093,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
   <ds:schemaRefs>

</xml_diff>